<commit_message>
Experimented with Other Losses and Optimizers
Tried optimizers LBFGS, Adam, RMSProp, Momentum, NAG, AdaMax

Tried losses Cross Entropy, Binary Cross Entropy, MSE, Hinge with ReLU/LeakyReLU/Tanh/Softmax
</commit_message>
<xml_diff>
--- a/Runtime Logs.xlsx
+++ b/Runtime Logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yuvraj\Projects\evol-rgap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D51E140-E016-43C1-AEE8-3D00A77A20CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D66B43D-67C7-4A1B-BDAD-312B63D3BC03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21540" windowHeight="7920" xr2:uid="{6952F2F2-0EDC-425B-8F4A-BDBACEF96FBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>S.No.</t>
   </si>
@@ -84,9 +84,6 @@
     <t>1 | 4.86</t>
   </si>
   <si>
-    <t>0.98 | 75.56</t>
-  </si>
-  <si>
     <t>0.97 | 104.44</t>
   </si>
   <si>
@@ -118,6 +115,21 @@
   </si>
   <si>
     <t>0.98 | 63.49</t>
+  </si>
+  <si>
+    <t>Cross-Entropy</t>
+  </si>
+  <si>
+    <t>Binary Cross-Entropy</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>0.99 | 72.89</t>
+  </si>
+  <si>
+    <t>0.97 | 90.91</t>
   </si>
 </sst>
 </file>
@@ -271,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -293,19 +305,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -622,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A884BC7-ADB9-4C3E-BE1B-2F8C9503DB91}">
-  <dimension ref="B3:F31"/>
+  <dimension ref="B3:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,27 +656,30 @@
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
@@ -840,22 +864,22 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="19" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+    <row r="19" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="7" t="s">
         <v>13</v>
       </c>
@@ -865,8 +889,17 @@
       <c r="F20" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>1</v>
       </c>
@@ -883,7 +916,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>2</v>
       </c>
@@ -891,16 +924,19 @@
         <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>3</v>
       </c>
@@ -908,16 +944,16 @@
         <v>26</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>4</v>
       </c>
@@ -925,16 +961,16 @@
         <v>52</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>5</v>
       </c>
@@ -942,16 +978,25 @@
         <v>387</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>6</v>
       </c>
@@ -960,7 +1005,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>7</v>
       </c>
@@ -969,7 +1014,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>8</v>
       </c>
@@ -978,7 +1023,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>9</v>
       </c>
@@ -987,7 +1032,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>10</v>
       </c>
@@ -996,7 +1041,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -1014,5 +1059,6 @@
     <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added More Objective Functions
Added more objective functions for DE - At Pop 7, Quantile is Goooood, Then log-cosh, Then MAE and Chebyshov
</commit_message>
<xml_diff>
--- a/Runtime Logs.xlsx
+++ b/Runtime Logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yuvraj\Projects\evol-rgap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D66B43D-67C7-4A1B-BDAD-312B63D3BC03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8647C63E-FD34-435B-A34A-59538C9D3081}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21540" windowHeight="7920" xr2:uid="{6952F2F2-0EDC-425B-8F4A-BDBACEF96FBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>S.No.</t>
   </si>
@@ -130,6 +130,78 @@
   </si>
   <si>
     <t>0.97 | 90.91</t>
+  </si>
+  <si>
+    <t>Exponential (R-GAP)</t>
+  </si>
+  <si>
+    <t>Hinge (R-GAP)</t>
+  </si>
+  <si>
+    <t>0.97 | 88.56</t>
+  </si>
+  <si>
+    <t>0.99 | 147.47</t>
+  </si>
+  <si>
+    <t>0.98 | 141.96</t>
+  </si>
+  <si>
+    <t>1 | 43.04</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Pop 10 - MSE - [-1:1, -5:5]</t>
+  </si>
+  <si>
+    <t>Pop 7 - Quantile - [-1:1]</t>
+  </si>
+  <si>
+    <t>0.99 | 5.95</t>
+  </si>
+  <si>
+    <t>0.98 | 51.54</t>
+  </si>
+  <si>
+    <t>0.99 | 123.76</t>
+  </si>
+  <si>
+    <t>0.99 | 111.266</t>
+  </si>
+  <si>
+    <t>1 | 22.69</t>
+  </si>
+  <si>
+    <t>1 | 4.68</t>
+  </si>
+  <si>
+    <t>0.98 | 48.42</t>
+  </si>
+  <si>
+    <t>0.99 | 133.97</t>
+  </si>
+  <si>
+    <t>0.99 | 100.52</t>
+  </si>
+  <si>
+    <t>1 | 25.67</t>
+  </si>
+  <si>
+    <t>1 | 20.06</t>
+  </si>
+  <si>
+    <t>1 | 3.98</t>
+  </si>
+  <si>
+    <t>0.98 | 50.21</t>
+  </si>
+  <si>
+    <t>0.99 | 141.34</t>
+  </si>
+  <si>
+    <t>0.98 | 135.15</t>
   </si>
 </sst>
 </file>
@@ -158,12 +230,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -283,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,9 +370,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -320,6 +395,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -327,6 +408,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -643,420 +742,548 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A884BC7-ADB9-4C3E-BE1B-2F8C9503DB91}">
-  <dimension ref="B3:I31"/>
+  <dimension ref="B3:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="7" t="s">
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="14"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>10</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>127.315</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="19">
         <v>122.623</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>126.455</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="20">
         <v>120.962</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>126.55500000000001</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="20">
         <v>120.729</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>26</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>126.101</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="20">
         <v>121.80500000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>52</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>125.873</v>
       </c>
-      <c r="F9" s="5">
+      <c r="G9" s="20">
         <v>120.807</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>387</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>125.679</v>
       </c>
-      <c r="F10" s="5">
+      <c r="G10" s="20">
         <v>122.163</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>7</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>111.851</v>
       </c>
-      <c r="F11" s="5">
+      <c r="G11" s="20">
         <v>104.512</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>8</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>109.502</v>
       </c>
-      <c r="F12" s="5">
+      <c r="G12" s="20">
         <v>106.533</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>9</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>5.5519999999999996</v>
       </c>
-      <c r="F13" s="5">
+      <c r="G13" s="20">
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>10</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>6.6769999999999996</v>
       </c>
-      <c r="F14" s="5">
+      <c r="G14" s="20">
         <v>1.2150000000000001</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="19" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="E19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="15"/>
       <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="7" t="s">
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="14"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="H20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="I20" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="J20" s="8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K20" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1">
         <v>0</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>2</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1">
         <v>5</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="H22" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>3</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1">
         <v>26</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>4</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="1">
         <v>52</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>5</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="1">
         <v>387</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="I25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>6</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>7</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>8</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="1">
+        <v>26</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>9</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="1">
+        <v>52</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>10</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="1">
+        <v>387</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>